<commit_message>
week 14 playoffs start
</commit_message>
<xml_diff>
--- a/Brown Munde 2023.xlsx
+++ b/Brown Munde 2023.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="80">
   <si>
     <t>Still Rollin'</t>
   </si>
@@ -52,37 +52,34 @@
     <t>BurgerBoyz</t>
   </si>
   <si>
-    <t>9-4-0</t>
-  </si>
-  <si>
-    <t>5-8-0</t>
-  </si>
-  <si>
-    <t>4-9-0</t>
-  </si>
-  <si>
-    <t>7-6-0</t>
-  </si>
-  <si>
-    <t>8-5-0</t>
-  </si>
-  <si>
-    <t>6-7-0</t>
-  </si>
-  <si>
-    <t>3-10-0</t>
-  </si>
-  <si>
-    <t>10-3-0</t>
-  </si>
-  <si>
-    <t>11-2-0</t>
-  </si>
-  <si>
-    <t>2-11-0</t>
-  </si>
-  <si>
-    <t>1-12-0</t>
+    <t>10-4-0</t>
+  </si>
+  <si>
+    <t>6-8-0</t>
+  </si>
+  <si>
+    <t>4-10-0</t>
+  </si>
+  <si>
+    <t>8-6-0</t>
+  </si>
+  <si>
+    <t>9-5-0</t>
+  </si>
+  <si>
+    <t>7-7-0</t>
+  </si>
+  <si>
+    <t>5-9-0</t>
+  </si>
+  <si>
+    <t>3-11-0</t>
+  </si>
+  <si>
+    <t>11-3-0</t>
+  </si>
+  <si>
+    <t>1-13-0</t>
   </si>
   <si>
     <t>Teams</t>
@@ -145,63 +142,63 @@
     <t>Change From Last Week</t>
   </si>
   <si>
+    <t>Prahlad Singh</t>
+  </si>
+  <si>
     <t>KASHYAP AShok</t>
   </si>
   <si>
-    <t>Prahlad Singh</t>
-  </si>
-  <si>
     <t>Krishna Padodara</t>
   </si>
   <si>
+    <t>Utkarsh Gupta</t>
+  </si>
+  <si>
     <t>Harman Brar</t>
   </si>
   <si>
-    <t>Utkarsh Gupta</t>
+    <t>Hayat Khan</t>
   </si>
   <si>
     <t>suraj bhalani</t>
   </si>
   <si>
+    <t>Sahir Sachdev</t>
+  </si>
+  <si>
     <t>Harshit Aggarwal</t>
   </si>
   <si>
-    <t>Sahir Sachdev</t>
-  </si>
-  <si>
-    <t>Hayat Khan</t>
-  </si>
-  <si>
     <t>Hark Nanda</t>
   </si>
   <si>
+    <t>↑2</t>
+  </si>
+  <si>
+    <t>↓1</t>
+  </si>
+  <si>
+    <t>↓6</t>
+  </si>
+  <si>
+    <t>↑8</t>
+  </si>
+  <si>
+    <t>↓8</t>
+  </si>
+  <si>
+    <t>↑6</t>
+  </si>
+  <si>
+    <t>↓3</t>
+  </si>
+  <si>
     <t>↑3</t>
   </si>
   <si>
-    <t>↓6</t>
-  </si>
-  <si>
-    <t>↑4</t>
-  </si>
-  <si>
     <t>0</t>
   </si>
   <si>
-    <t>↑2</t>
-  </si>
-  <si>
-    <t>↓3</t>
-  </si>
-  <si>
-    <t>↑6</t>
-  </si>
-  <si>
-    <t>↓9</t>
-  </si>
-  <si>
-    <t>↑1</t>
-  </si>
-  <si>
     <t>Week 1</t>
   </si>
   <si>
@@ -239,6 +236,9 @@
   </si>
   <si>
     <t>Week 13</t>
+  </si>
+  <si>
+    <t>Week 14</t>
   </si>
   <si>
     <t>Week</t>
@@ -666,13 +666,13 @@
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G2" t="s">
         <v>10</v>
@@ -681,7 +681,7 @@
         <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J2" t="s">
         <v>15</v>
@@ -707,7 +707,7 @@
         <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
         <v>13</v>
@@ -719,10 +719,10 @@
         <v>10</v>
       </c>
       <c r="J3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="K3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -733,7 +733,7 @@
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
         <v>13</v>
@@ -742,7 +742,7 @@
         <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G4" t="s">
         <v>11</v>
@@ -754,10 +754,10 @@
         <v>15</v>
       </c>
       <c r="J4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="K4" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -768,19 +768,19 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
         <v>13</v>
       </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
@@ -789,10 +789,10 @@
         <v>15</v>
       </c>
       <c r="J5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="K5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -803,31 +803,31 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="G6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H6" t="s">
         <v>11</v>
       </c>
       <c r="I6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="J6" t="s">
         <v>12</v>
       </c>
       <c r="K6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -838,31 +838,31 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
         <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-      <c r="F7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" t="s">
-        <v>11</v>
       </c>
       <c r="H7" t="s">
         <v>11</v>
       </c>
       <c r="I7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" t="s">
         <v>11</v>
-      </c>
-      <c r="K7" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -876,28 +876,28 @@
         <v>13</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="H8" t="s">
         <v>14</v>
       </c>
       <c r="I8" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="J8" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="K8" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -905,34 +905,34 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" t="s">
         <v>13</v>
       </c>
-      <c r="C9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" t="s">
-        <v>17</v>
-      </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>14</v>
       </c>
-      <c r="G9" t="s">
-        <v>10</v>
-      </c>
       <c r="H9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="I9" t="s">
         <v>18</v>
       </c>
       <c r="J9" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" t="s">
         <v>15</v>
-      </c>
-      <c r="K9" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -940,34 +940,34 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
         <v>16</v>
-      </c>
-      <c r="D10" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" t="s">
-        <v>12</v>
       </c>
       <c r="F10" t="s">
         <v>12</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I10" t="s">
         <v>15</v>
       </c>
       <c r="J10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -987,7 +987,7 @@
         <v>14</v>
       </c>
       <c r="F11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G11" t="s">
         <v>14</v>
@@ -999,7 +999,7 @@
         <v>13</v>
       </c>
       <c r="J11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="K11" t="s">
         <v>11</v>
@@ -1020,13 +1020,13 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1037,10 +1037,10 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>4.8</v>
+        <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1051,7 +1051,7 @@
         <v>1</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>5.7</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -1065,7 +1065,7 @@
         <v>9</v>
       </c>
       <c r="C4">
-        <v>5.8</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
@@ -1079,7 +1079,7 @@
         <v>0</v>
       </c>
       <c r="C5">
-        <v>5.9</v>
+        <v>6.7</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -1093,7 +1093,7 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>6.9</v>
       </c>
       <c r="D6" t="s">
         <v>14</v>
@@ -1107,10 +1107,10 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>6.9</v>
+        <v>7.4</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1121,7 +1121,7 @@
         <v>2</v>
       </c>
       <c r="C8">
-        <v>7.2</v>
+        <v>7.7</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
@@ -1132,13 +1132,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C9">
-        <v>7.7</v>
+        <v>7.9</v>
       </c>
       <c r="D9" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1146,13 +1146,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C10">
-        <v>7.8</v>
+        <v>8.1</v>
       </c>
       <c r="D10" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1163,7 +1163,7 @@
         <v>7</v>
       </c>
       <c r="C11">
-        <v>7.9</v>
+        <v>8.6</v>
       </c>
       <c r="D11" t="s">
         <v>18</v>
@@ -1184,16 +1184,16 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="B1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1201,16 +1201,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>8.4</v>
+        <v>9.4</v>
       </c>
       <c r="D2">
-        <v>-2.6</v>
+        <v>-0.5999999999999996</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -1218,16 +1218,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C3">
-        <v>8.4</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="D3">
-        <v>-0.5999999999999996</v>
+        <v>-0.1999999999999993</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -1235,16 +1235,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>8.4</v>
       </c>
       <c r="D4">
-        <v>0.4000000000000004</v>
+        <v>-2.6</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1255,10 +1255,10 @@
         <v>1</v>
       </c>
       <c r="C5">
-        <v>7.6</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="D5">
-        <v>0.5999999999999996</v>
+        <v>0.1999999999999993</v>
       </c>
       <c r="E5" t="s">
         <v>13</v>
@@ -1269,16 +1269,16 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="C6">
-        <v>6.4</v>
+        <v>7.2</v>
       </c>
       <c r="D6">
-        <v>-0.5999999999999996</v>
+        <v>1.2</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1286,16 +1286,16 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C7">
-        <v>6.3</v>
+        <v>6.8</v>
       </c>
       <c r="D7">
-        <v>1.3</v>
+        <v>-0.2000000000000002</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -1303,16 +1303,16 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C8">
-        <v>6</v>
+        <v>6.5</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>-1.5</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1320,16 +1320,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C9">
-        <v>5.8</v>
+        <v>6.2</v>
       </c>
       <c r="D9">
-        <v>-1.2</v>
+        <v>1.2</v>
       </c>
       <c r="E9" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1340,13 +1340,13 @@
         <v>4</v>
       </c>
       <c r="C10">
-        <v>4.3</v>
+        <v>4.4</v>
       </c>
       <c r="D10">
-        <v>-0.7000000000000002</v>
+        <v>-0.5999999999999996</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1357,13 +1357,13 @@
         <v>8</v>
       </c>
       <c r="C11">
-        <v>3.4</v>
+        <v>4.1</v>
       </c>
       <c r="D11">
-        <v>2.4</v>
+        <v>3.1</v>
       </c>
       <c r="E11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1381,40 +1381,40 @@
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -1422,10 +1422,10 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>25.77</v>
+        <v>23.81</v>
       </c>
       <c r="C2">
-        <v>3.54</v>
+        <v>3.56</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -1437,10 +1437,10 @@
         <v>0</v>
       </c>
       <c r="G2">
-        <v>13.93</v>
+        <v>17.02</v>
       </c>
       <c r="H2">
-        <v>56.76</v>
+        <v>55.61000000000001</v>
       </c>
       <c r="I2">
         <v>0</v>
@@ -1452,7 +1452,7 @@
         <v>0</v>
       </c>
       <c r="L2">
-        <v>43.24</v>
+        <v>44.39</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -1460,13 +1460,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>23.04</v>
+        <v>22.96</v>
       </c>
       <c r="C3">
-        <v>10.05</v>
+        <v>10.92</v>
       </c>
       <c r="D3">
-        <v>0.58</v>
+        <v>0.46</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -1475,13 +1475,13 @@
         <v>0</v>
       </c>
       <c r="G3">
-        <v>2.96</v>
+        <v>3.1</v>
       </c>
       <c r="H3">
-        <v>29.65</v>
+        <v>29.91</v>
       </c>
       <c r="I3">
-        <v>33.72</v>
+        <v>32.65</v>
       </c>
       <c r="J3">
         <v>0</v>
@@ -1490,121 +1490,121 @@
         <v>0</v>
       </c>
       <c r="L3">
-        <v>36.63</v>
+        <v>37.44</v>
       </c>
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>19.91</v>
+        <v>20.58</v>
       </c>
       <c r="C4">
-        <v>20.61</v>
+        <v>0</v>
       </c>
       <c r="D4">
-        <v>3.21</v>
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0.06999999999999999</v>
+        <v>0</v>
       </c>
       <c r="F4">
         <v>0</v>
       </c>
       <c r="G4">
-        <v>0.51</v>
+        <v>79.42</v>
       </c>
       <c r="H4">
-        <v>9.800000000000001</v>
+        <v>0</v>
       </c>
       <c r="I4">
-        <v>32.08</v>
+        <v>0</v>
       </c>
       <c r="J4">
-        <v>13.81</v>
+        <v>0</v>
       </c>
       <c r="K4">
         <v>0</v>
       </c>
       <c r="L4">
-        <v>44.31</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>17.47</v>
+        <v>20.44</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>23.72</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>4.16</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="F5">
         <v>0</v>
       </c>
       <c r="G5">
-        <v>82.53</v>
+        <v>0.4</v>
       </c>
       <c r="H5">
-        <v>0</v>
+        <v>9.859999999999999</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>29.15</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>12.21</v>
       </c>
       <c r="K5">
         <v>0</v>
       </c>
       <c r="L5">
-        <v>100</v>
+        <v>48.77999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B6">
-        <v>10.73</v>
+        <v>9.69</v>
       </c>
       <c r="C6">
-        <v>28.68</v>
+        <v>27.18</v>
       </c>
       <c r="D6">
-        <v>10.67</v>
+        <v>12.03</v>
       </c>
       <c r="E6">
-        <v>0.79</v>
+        <v>0.8200000000000001</v>
       </c>
       <c r="F6">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="G6">
         <v>0.06</v>
       </c>
       <c r="H6">
-        <v>2.93</v>
+        <v>3.74</v>
       </c>
       <c r="I6">
-        <v>19.74</v>
+        <v>21.55</v>
       </c>
       <c r="J6">
-        <v>23.31</v>
+        <v>22.41</v>
       </c>
       <c r="K6">
-        <v>3.08</v>
+        <v>2.52</v>
       </c>
       <c r="L6">
-        <v>50.94</v>
+        <v>49.78</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -1612,37 +1612,37 @@
         <v>3</v>
       </c>
       <c r="B7">
-        <v>3.08</v>
+        <v>2.52</v>
       </c>
       <c r="C7">
-        <v>24.91</v>
+        <v>23.18</v>
       </c>
       <c r="D7">
-        <v>23.47</v>
+        <v>23.24</v>
       </c>
       <c r="E7">
-        <v>3.66</v>
+        <v>4.31</v>
       </c>
       <c r="F7">
-        <v>0.1</v>
+        <v>0.06999999999999999</v>
       </c>
       <c r="G7">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="H7">
-        <v>0.75</v>
+        <v>0.8099999999999999</v>
       </c>
       <c r="I7">
-        <v>9.94</v>
+        <v>11.46</v>
       </c>
       <c r="J7">
-        <v>24.95</v>
+        <v>25.49</v>
       </c>
       <c r="K7">
-        <v>9.130000000000001</v>
+        <v>8.92</v>
       </c>
       <c r="L7">
-        <v>55.23</v>
+        <v>53.32</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -1653,39 +1653,39 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>12.21</v>
+        <v>11.44</v>
       </c>
       <c r="D8">
-        <v>35.96</v>
+        <v>34.75</v>
       </c>
       <c r="E8">
-        <v>14.76</v>
+        <v>14.99</v>
       </c>
       <c r="F8">
-        <v>1.1</v>
+        <v>0.8999999999999999</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
       <c r="H8">
-        <v>0.11</v>
+        <v>0.06999999999999999</v>
       </c>
       <c r="I8">
-        <v>3.31</v>
+        <v>4.22</v>
       </c>
       <c r="J8">
-        <v>18.65</v>
+        <v>19.71</v>
       </c>
       <c r="K8">
-        <v>13.9</v>
+        <v>13.92</v>
       </c>
       <c r="L8">
-        <v>64.03</v>
+        <v>62.08</v>
       </c>
     </row>
     <row r="9" spans="1:12">
       <c r="A9" s="1" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -1694,13 +1694,13 @@
         <v>0</v>
       </c>
       <c r="D9">
-        <v>26.11</v>
+        <v>25.36</v>
       </c>
       <c r="E9">
-        <v>35.15</v>
+        <v>32.02999999999999</v>
       </c>
       <c r="F9">
-        <v>5.64</v>
+        <v>4.22</v>
       </c>
       <c r="G9">
         <v>0</v>
@@ -1709,21 +1709,21 @@
         <v>0</v>
       </c>
       <c r="I9">
-        <v>1.21</v>
+        <v>0.97</v>
       </c>
       <c r="J9">
-        <v>12.43</v>
+        <v>14.99</v>
       </c>
       <c r="K9">
-        <v>19.46</v>
+        <v>22.43</v>
       </c>
       <c r="L9">
-        <v>66.89999999999999</v>
+        <v>61.60999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -1735,10 +1735,10 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>45.57</v>
+        <v>47.79</v>
       </c>
       <c r="F10">
-        <v>21.73</v>
+        <v>16.67</v>
       </c>
       <c r="G10">
         <v>0</v>
@@ -1750,13 +1750,13 @@
         <v>0</v>
       </c>
       <c r="J10">
-        <v>6.850000000000001</v>
+        <v>5.19</v>
       </c>
       <c r="K10">
-        <v>25.85</v>
+        <v>30.35</v>
       </c>
       <c r="L10">
-        <v>67.3</v>
+        <v>64.45999999999999</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -1776,7 +1776,7 @@
         <v>0</v>
       </c>
       <c r="F11">
-        <v>71.41999999999999</v>
+        <v>78.14</v>
       </c>
       <c r="G11">
         <v>0</v>
@@ -1791,10 +1791,10 @@
         <v>0</v>
       </c>
       <c r="K11">
-        <v>28.58</v>
+        <v>21.86</v>
       </c>
       <c r="L11">
-        <v>71.41999999999999</v>
+        <v>78.14</v>
       </c>
     </row>
   </sheetData>
@@ -1812,19 +1812,19 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1832,19 +1832,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1852,19 +1852,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D3">
         <v>30</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1875,16 +1875,16 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D4">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E4" t="s">
         <v>14</v>
       </c>
       <c r="F4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1892,19 +1892,19 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -1912,19 +1912,19 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D6">
-        <v>6</v>
+        <v>-2</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1932,19 +1932,19 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D7">
         <v>-11</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1952,19 +1952,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D8">
-        <v>-16</v>
+        <v>-14</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1975,16 +1975,16 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D9">
-        <v>-17</v>
+        <v>-14</v>
       </c>
       <c r="E9" t="s">
         <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1992,19 +1992,19 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D10">
-        <v>-17</v>
+        <v>-16</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -2015,16 +2015,16 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11">
         <v>-42</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F11" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2034,151 +2034,160 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:16">
       <c r="B1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15">
+      <c r="P1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2">
+        <v>8</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>7</v>
-      </c>
-      <c r="D2">
-        <v>13</v>
-      </c>
-      <c r="E2">
+      <c r="H2">
+        <v>14</v>
+      </c>
+      <c r="I2">
+        <v>22</v>
+      </c>
+      <c r="J2">
         <v>24</v>
-      </c>
-      <c r="F2">
-        <v>31</v>
-      </c>
-      <c r="G2">
-        <v>28</v>
-      </c>
-      <c r="H2">
-        <v>26</v>
-      </c>
-      <c r="I2">
-        <v>25</v>
-      </c>
-      <c r="J2">
-        <v>19</v>
       </c>
       <c r="K2">
         <v>24</v>
       </c>
       <c r="L2">
+        <v>32</v>
+      </c>
+      <c r="M2">
+        <v>36</v>
+      </c>
+      <c r="N2">
+        <v>30</v>
+      </c>
+      <c r="O2">
+        <v>32</v>
+      </c>
+      <c r="P2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>13</v>
+      </c>
+      <c r="E3">
+        <v>24</v>
+      </c>
+      <c r="F3">
+        <v>31</v>
+      </c>
+      <c r="G3">
         <v>28</v>
       </c>
-      <c r="M2">
-        <v>28</v>
-      </c>
-      <c r="N2">
-        <v>31</v>
-      </c>
-      <c r="O2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15">
-      <c r="A3" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>10</v>
-      </c>
-      <c r="D3">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3">
-        <v>5</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
       <c r="H3">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="I3">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="J3">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="K3">
         <v>24</v>
       </c>
       <c r="L3">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="M3">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="N3">
+        <v>31</v>
+      </c>
+      <c r="O3">
         <v>30</v>
       </c>
-      <c r="O3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15">
+      <c r="P3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -2221,199 +2230,214 @@
       <c r="N4">
         <v>29</v>
       </c>
-      <c r="O4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15">
+      <c r="O4">
+        <v>23</v>
+      </c>
+      <c r="P4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
       <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>-1</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>6</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
         <v>7</v>
       </c>
-      <c r="B5">
-        <v>-6</v>
-      </c>
-      <c r="C5">
-        <v>-11</v>
-      </c>
-      <c r="D5">
-        <v>-2</v>
-      </c>
-      <c r="E5">
-        <v>-7</v>
-      </c>
-      <c r="F5">
-        <v>-2</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>-5</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
       <c r="J5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="K5">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="L5">
+        <v>6</v>
+      </c>
+      <c r="M5">
         <v>4</v>
-      </c>
-      <c r="M5">
-        <v>6</v>
       </c>
       <c r="N5">
         <v>6</v>
       </c>
-      <c r="O5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15">
+      <c r="O5">
+        <v>14</v>
+      </c>
+      <c r="P5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
       <c r="A6" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>-1</v>
+        <v>-6</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>-11</v>
       </c>
       <c r="D6">
+        <v>-2</v>
+      </c>
+      <c r="E6">
+        <v>-7</v>
+      </c>
+      <c r="F6">
+        <v>-2</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>-5</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>7</v>
+      </c>
+      <c r="K6">
+        <v>14</v>
+      </c>
+      <c r="L6">
+        <v>4</v>
+      </c>
+      <c r="M6">
         <v>6</v>
-      </c>
-      <c r="E6">
-        <v>4</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>6</v>
-      </c>
-      <c r="H6">
-        <v>4</v>
-      </c>
-      <c r="I6">
-        <v>7</v>
-      </c>
-      <c r="J6">
-        <v>4</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>6</v>
-      </c>
-      <c r="M6">
-        <v>4</v>
       </c>
       <c r="N6">
         <v>6</v>
       </c>
-      <c r="O6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15">
+      <c r="O6">
+        <v>-2</v>
+      </c>
+      <c r="P6" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>-6</v>
       </c>
       <c r="D7">
+        <v>-7</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>-5</v>
+      </c>
+      <c r="G7">
+        <v>-2</v>
+      </c>
+      <c r="H7">
+        <v>-4</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+      <c r="J7">
+        <v>6</v>
+      </c>
+      <c r="K7">
         <v>-1</v>
-      </c>
-      <c r="E7">
-        <v>-4</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>6</v>
-      </c>
-      <c r="H7">
-        <v>14</v>
-      </c>
-      <c r="I7">
-        <v>6</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>-6</v>
       </c>
       <c r="L7">
         <v>-10</v>
       </c>
       <c r="M7">
-        <v>-8</v>
+        <v>-18</v>
       </c>
       <c r="N7">
+        <v>-17</v>
+      </c>
+      <c r="O7">
         <v>-11</v>
       </c>
-      <c r="O7" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15">
+      <c r="P7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
       <c r="A8" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B8">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C8">
+        <v>2</v>
+      </c>
+      <c r="D8">
         <v>-1</v>
-      </c>
-      <c r="D8">
-        <v>-2</v>
       </c>
       <c r="E8">
         <v>-4</v>
       </c>
       <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>6</v>
+      </c>
+      <c r="H8">
+        <v>14</v>
+      </c>
+      <c r="I8">
+        <v>6</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>-6</v>
+      </c>
+      <c r="L8">
+        <v>-10</v>
+      </c>
+      <c r="M8">
         <v>-8</v>
       </c>
-      <c r="G8">
-        <v>-8</v>
-      </c>
-      <c r="H8">
-        <v>-12</v>
-      </c>
-      <c r="I8">
-        <v>-18</v>
-      </c>
-      <c r="J8">
-        <v>-18</v>
-      </c>
-      <c r="K8">
-        <v>-23</v>
-      </c>
-      <c r="L8">
-        <v>-22</v>
-      </c>
-      <c r="M8">
-        <v>-22</v>
-      </c>
       <c r="N8">
-        <v>-16</v>
-      </c>
-      <c r="O8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15">
+        <v>-11</v>
+      </c>
+      <c r="O8">
+        <v>-14</v>
+      </c>
+      <c r="P8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
@@ -2456,58 +2480,64 @@
       <c r="N9">
         <v>-17</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O9">
+        <v>-14</v>
+      </c>
+      <c r="P9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10">
+        <v>-1</v>
+      </c>
+      <c r="D10">
+        <v>-2</v>
+      </c>
+      <c r="E10">
+        <v>-4</v>
+      </c>
+      <c r="F10">
+        <v>-8</v>
+      </c>
+      <c r="G10">
+        <v>-8</v>
+      </c>
+      <c r="H10">
+        <v>-12</v>
+      </c>
+      <c r="I10">
+        <v>-18</v>
+      </c>
+      <c r="J10">
+        <v>-18</v>
+      </c>
+      <c r="K10">
+        <v>-23</v>
+      </c>
+      <c r="L10">
+        <v>-22</v>
+      </c>
+      <c r="M10">
+        <v>-22</v>
+      </c>
+      <c r="N10">
+        <v>-16</v>
+      </c>
+      <c r="O10">
+        <v>-16</v>
+      </c>
+      <c r="P10" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:15">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>-6</v>
-      </c>
-      <c r="D10">
-        <v>-7</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>-5</v>
-      </c>
-      <c r="G10">
-        <v>-2</v>
-      </c>
-      <c r="H10">
-        <v>-4</v>
-      </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-      <c r="J10">
-        <v>6</v>
-      </c>
-      <c r="K10">
-        <v>-1</v>
-      </c>
-      <c r="L10">
-        <v>-10</v>
-      </c>
-      <c r="M10">
-        <v>-18</v>
-      </c>
-      <c r="N10">
-        <v>-17</v>
-      </c>
-      <c r="O10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:16">
       <c r="A11" s="1" t="s">
         <v>4</v>
       </c>
@@ -2550,8 +2580,11 @@
       <c r="N11">
         <v>-42</v>
       </c>
-      <c r="O11" t="s">
-        <v>54</v>
+      <c r="O11">
+        <v>-42</v>
+      </c>
+      <c r="P11" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -2561,7 +2594,7 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2876,58 +2909,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="1">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>3</v>
-      </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>-2</v>
-      </c>
-      <c r="F13">
-        <v>13</v>
-      </c>
-      <c r="G13">
-        <v>15</v>
-      </c>
-      <c r="H13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="1">
-        <v>12</v>
-      </c>
-      <c r="B14">
-        <v>6</v>
-      </c>
-      <c r="C14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" t="s">
-        <v>4</v>
-      </c>
-      <c r="E14">
-        <v>-28</v>
-      </c>
-      <c r="F14">
-        <v>-13</v>
-      </c>
-      <c r="G14">
-        <v>15</v>
-      </c>
-      <c r="H14" t="s">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>